<commit_message>
merged from eroots devel
</commit_message>
<xml_diff>
--- a/src/tests/data/results/IEEE 30 bus.sav.xlsx
+++ b/src/tests/data/results/IEEE 30 bus.sav.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Vabs" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Vang" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Pbranch" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Qbranch" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Vabs" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Vang" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Pbranch" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Qbranch" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Qgen" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
   <si>
     <t xml:space="preserve">1</t>
   </si>
@@ -239,6 +240,9 @@
   </si>
   <si>
     <t xml:space="preserve">27_28_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVAr</t>
   </si>
 </sst>
 </file>
@@ -329,13 +333,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -350,15 +358,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:B42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,7 +486,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>1.05999994277954</v>
       </c>
     </row>
@@ -380,7 +494,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>1.04499991168836</v>
       </c>
     </row>
@@ -388,7 +502,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>1.02117763781835</v>
       </c>
     </row>
@@ -396,7 +510,7 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>1.01230036792654</v>
       </c>
     </row>
@@ -404,7 +518,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>1.00999999249818</v>
       </c>
     </row>
@@ -412,7 +526,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>1.01062570429387</v>
       </c>
     </row>
@@ -420,7 +534,7 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>1.00259705029173</v>
       </c>
     </row>
@@ -428,7 +542,7 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>1.00999998129108</v>
       </c>
     </row>
@@ -436,7 +550,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>1.05113165464091</v>
       </c>
     </row>
@@ -444,7 +558,7 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>1.04537889818895</v>
       </c>
     </row>
@@ -452,7 +566,7 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>1.08199996535958</v>
       </c>
     </row>
@@ -460,7 +574,7 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>1.05733885405535</v>
       </c>
     </row>
@@ -468,7 +582,7 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <v>1.07100002040524</v>
       </c>
     </row>
@@ -476,7 +590,7 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="2" t="n">
         <v>1.04250773898323</v>
       </c>
     </row>
@@ -484,7 +598,7 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <v>1.03791587573137</v>
       </c>
     </row>
@@ -492,7 +606,7 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="2" t="n">
         <v>1.04462582784323</v>
       </c>
     </row>
@@ -500,7 +614,7 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="2" t="n">
         <v>1.0401502793489</v>
       </c>
     </row>
@@ -508,7 +622,7 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="2" t="n">
         <v>1.02839626742803</v>
       </c>
     </row>
@@ -516,7 +630,7 @@
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="2" t="n">
         <v>1.02589994495438</v>
       </c>
     </row>
@@ -524,7 +638,7 @@
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="2" t="n">
         <v>1.029986687839</v>
       </c>
     </row>
@@ -532,7 +646,7 @@
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="2" t="n">
         <v>1.03298218678066</v>
       </c>
     </row>
@@ -540,7 +654,7 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="2" t="n">
         <v>1.03351363328317</v>
       </c>
     </row>
@@ -548,7 +662,7 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="2" t="n">
         <v>1.02742897975398</v>
       </c>
     </row>
@@ -556,7 +670,7 @@
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="2" t="n">
         <v>1.02184577612474</v>
       </c>
     </row>
@@ -564,7 +678,7 @@
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="2" t="n">
         <v>1.01761861718844</v>
       </c>
     </row>
@@ -572,7 +686,7 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="2" t="n">
         <v>0.999946367387374</v>
       </c>
     </row>
@@ -580,7 +694,7 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="2" t="n">
         <v>1.0235384780157</v>
       </c>
     </row>
@@ -588,7 +702,7 @@
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="2" t="n">
         <v>1.00710102233856</v>
       </c>
     </row>
@@ -596,7 +710,7 @@
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="2" t="n">
         <v>1.0037057741359</v>
       </c>
     </row>
@@ -604,7 +718,7 @@
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="2" t="n">
         <v>0.992234779674377</v>
       </c>
     </row>
@@ -620,14 +734,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:B42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -641,7 +755,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -649,7 +763,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>-0.0938680675279496</v>
       </c>
     </row>
@@ -657,7 +771,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>-0.131399914355754</v>
       </c>
     </row>
@@ -665,7 +779,7 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>-0.161956674411848</v>
       </c>
     </row>
@@ -673,7 +787,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>-0.246942610345029</v>
       </c>
     </row>
@@ -681,7 +795,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>-0.192946583491403</v>
       </c>
     </row>
@@ -689,7 +803,7 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>-0.224315306945025</v>
       </c>
     </row>
@@ -697,7 +811,7 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>-0.205903251917542</v>
       </c>
     </row>
@@ -705,7 +819,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>-0.246056021035836</v>
       </c>
     </row>
@@ -713,7 +827,7 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>-0.27381033443421</v>
       </c>
     </row>
@@ -721,7 +835,7 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>-0.246056014716265</v>
       </c>
     </row>
@@ -729,7 +843,7 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>-0.260628447856205</v>
       </c>
     </row>
@@ -737,7 +851,7 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <v>-0.260628441726585</v>
       </c>
     </row>
@@ -745,7 +859,7 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="2" t="n">
         <v>-0.276190055976999</v>
       </c>
     </row>
@@ -753,7 +867,7 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <v>-0.277792981669785</v>
       </c>
     </row>
@@ -761,7 +875,7 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="2" t="n">
         <v>-0.270795276358074</v>
       </c>
     </row>
@@ -769,7 +883,7 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="2" t="n">
         <v>-0.276633809267762</v>
       </c>
     </row>
@@ -777,7 +891,7 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="2" t="n">
         <v>-0.288506256058098</v>
       </c>
     </row>
@@ -785,7 +899,7 @@
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="2" t="n">
         <v>-0.291534982130216</v>
       </c>
     </row>
@@ -793,7 +907,7 @@
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="2" t="n">
         <v>-0.288104899606405</v>
       </c>
     </row>
@@ -801,7 +915,7 @@
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="2" t="n">
         <v>-0.281533267004714</v>
       </c>
     </row>
@@ -809,7 +923,7 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="2" t="n">
         <v>-0.281284928888078</v>
       </c>
     </row>
@@ -817,7 +931,7 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="2" t="n">
         <v>-0.284604342956748</v>
       </c>
     </row>
@@ -825,7 +939,7 @@
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="2" t="n">
         <v>-0.287678926455809</v>
       </c>
     </row>
@@ -833,7 +947,7 @@
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="2" t="n">
         <v>-0.28020495305378</v>
       </c>
     </row>
@@ -841,7 +955,7 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="2" t="n">
         <v>-0.287525237336158</v>
       </c>
     </row>
@@ -849,7 +963,7 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="2" t="n">
         <v>-0.271051067338068</v>
       </c>
     </row>
@@ -857,7 +971,7 @@
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="2" t="n">
         <v>-0.203807299206197</v>
       </c>
     </row>
@@ -865,7 +979,7 @@
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="2" t="n">
         <v>-0.292505231621384</v>
       </c>
     </row>
@@ -873,7 +987,7 @@
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="2" t="n">
         <v>-0.307904281470447</v>
       </c>
     </row>
@@ -889,19 +1003,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="25.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,330 +1024,330 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>173.30714</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>87.6498</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>43.65269</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>82.36132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>60.37998</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>82.1419</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>72.12732</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>-14.78171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>38.13212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>29.56305</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>18.6735</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>-0.54496</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <v>5.33167</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="2" t="n">
         <v>9.02535</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <v>15.78559</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="2" t="n">
         <v>7.6183</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="2" t="n">
         <v>7.85752</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="2" t="n">
         <v>17.89177</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="2" t="n">
         <v>7.24394</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="2" t="n">
         <v>1.58319</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="2" t="n">
         <v>6.01683</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="2" t="n">
         <v>5.03533</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="2" t="n">
         <v>3.6901</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="2" t="n">
         <v>2.77823</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="2" t="n">
         <v>-6.72666</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="2" t="n">
         <v>-1.82568</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="2" t="n">
         <v>5.73935</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="2" t="n">
         <v>1.80394</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="2" t="n">
         <v>-1.20827</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="2" t="n">
         <v>3.54463</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="2" t="n">
         <v>-4.76285</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="2" t="n">
         <v>6.18995</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="2" t="n">
         <v>7.092</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="2" t="n">
         <v>3.70371</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="2" t="n">
         <v>44.19323</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="2" t="n">
         <v>27.72124</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="2" t="n">
         <v>15.83966</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="2" t="n">
         <v>18.06888</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="2" t="n">
         <v>27.72125</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1249,14 +1363,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:B42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1270,7 +1384,7 @@
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>-24.7027912139893</v>
       </c>
     </row>
@@ -1278,7 +1392,7 @@
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>4.28486967086792</v>
       </c>
     </row>
@@ -1286,7 +1400,7 @@
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>4.74956703186035</v>
       </c>
     </row>
@@ -1294,7 +1408,7 @@
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>2.78163409233093</v>
       </c>
     </row>
@@ -1302,7 +1416,7 @@
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>1.37238574028015</v>
       </c>
     </row>
@@ -1310,7 +1424,7 @@
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>-3.85462784767151</v>
       </c>
     </row>
@@ -1318,7 +1432,7 @@
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>-15.9120197296143</v>
       </c>
     </row>
@@ -1326,7 +1440,7 @@
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>11.4903240203857</v>
       </c>
     </row>
@@ -1334,7 +1448,7 @@
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>-2.78136515617371</v>
       </c>
     </row>
@@ -1342,7 +1456,7 @@
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>-7.19653463363647</v>
       </c>
     </row>
@@ -1350,7 +1464,7 @@
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>0.114676266908646</v>
       </c>
     </row>
@@ -1358,7 +1472,7 @@
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>-0.544621825218201</v>
       </c>
     </row>
@@ -1366,7 +1480,7 @@
       <c r="A14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <v>5.88191223144531</v>
       </c>
     </row>
@@ -1374,7 +1488,7 @@
       <c r="A15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="2" t="n">
         <v>-15.5993537902832</v>
       </c>
     </row>
@@ -1382,7 +1496,7 @@
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <v>4.42940664291382</v>
       </c>
     </row>
@@ -1390,7 +1504,7 @@
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="2" t="n">
         <v>3.70956254005432</v>
       </c>
     </row>
@@ -1398,7 +1512,7 @@
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="2" t="n">
         <v>10.0108547210693</v>
       </c>
     </row>
@@ -1406,7 +1520,7 @@
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="2" t="n">
         <v>4.60002613067627</v>
       </c>
     </row>
@@ -1414,7 +1528,7 @@
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="2" t="n">
         <v>-10.3174180984497</v>
       </c>
     </row>
@@ -1422,7 +1536,7 @@
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="2" t="n">
         <v>2.40030479431152</v>
       </c>
     </row>
@@ -1430,7 +1544,7 @@
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="2" t="n">
         <v>6.7899169921875</v>
       </c>
     </row>
@@ -1438,7 +1552,7 @@
       <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="2" t="n">
         <v>3.3485643863678</v>
       </c>
     </row>
@@ -1446,7 +1560,7 @@
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="2" t="n">
         <v>0.645794153213501</v>
       </c>
     </row>
@@ -1454,7 +1568,7 @@
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="2" t="n">
         <v>1.59529912471771</v>
       </c>
     </row>
@@ -1462,7 +1576,7 @@
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="2" t="n">
         <v>2.90788221359253</v>
       </c>
     </row>
@@ -1470,7 +1584,7 @@
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="2" t="n">
         <v>1.43537056446075</v>
       </c>
     </row>
@@ -1478,7 +1592,7 @@
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="2" t="n">
         <v>0.616709232330322</v>
       </c>
     </row>
@@ -1486,7 +1600,7 @@
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="2" t="n">
         <v>-2.79318451881409</v>
       </c>
     </row>
@@ -1494,7 +1608,7 @@
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="2" t="n">
         <v>-1.42861878871918</v>
       </c>
     </row>
@@ -1502,7 +1616,7 @@
       <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="2" t="n">
         <v>3.06158328056335</v>
       </c>
     </row>
@@ -1510,7 +1624,7 @@
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="2" t="n">
         <v>1.24448418617248</v>
       </c>
     </row>
@@ -1518,7 +1632,7 @@
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="2" t="n">
         <v>2.01279997825623</v>
       </c>
     </row>
@@ -1526,7 +1640,7 @@
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="2" t="n">
         <v>2.36665916442871</v>
       </c>
     </row>
@@ -1534,7 +1648,7 @@
       <c r="A35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="2" t="n">
         <v>-0.371234387159347</v>
       </c>
     </row>
@@ -1542,7 +1656,7 @@
       <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="2" t="n">
         <v>1.66878843307495</v>
       </c>
     </row>
@@ -1550,7 +1664,7 @@
       <c r="A37" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="2" t="n">
         <v>1.66277551651001</v>
       </c>
     </row>
@@ -1558,7 +1672,7 @@
       <c r="A38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="2" t="n">
         <v>0.605859696865082</v>
       </c>
     </row>
@@ -1566,7 +1680,7 @@
       <c r="A39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="2" t="n">
         <v>14.4100160598755</v>
       </c>
     </row>
@@ -1574,7 +1688,7 @@
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="2" t="n">
         <v>-8.09298419952393</v>
       </c>
     </row>
@@ -1582,7 +1696,7 @@
       <c r="A41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="2" t="n">
         <v>0.186543717980385</v>
       </c>
     </row>
@@ -1590,7 +1704,7 @@
       <c r="A42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="2" t="n">
         <v>-3.74879360198975</v>
       </c>
     </row>
@@ -1603,4 +1717,81 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>-20.4176</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>56.0691</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>35.6585</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>36.111</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>16.0574</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>10.4507</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>